<commit_message>
Use Cell Format, When output to string.
</commit_message>
<xml_diff>
--- a/testdoc1/test1.xlsx
+++ b/testdoc1/test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="シート1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>日本語</t>
     <rPh sb="0" eb="3">
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>どうかな</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>改行つき
 どうかな?</t>
     <rPh sb="0" eb="2">
@@ -153,6 +149,41 @@
     <t>那覇</t>
     <rPh sb="0" eb="2">
       <t>ナハ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>日付</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>数字</t>
+    <rPh sb="0" eb="2">
+      <t>スウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>通貨</t>
+    <rPh sb="0" eb="2">
+      <t>ツウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>会計</t>
+    <rPh sb="0" eb="2">
+      <t>カイケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>時刻</t>
+    <rPh sb="0" eb="2">
+      <t>ジコク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -161,6 +192,61 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="53">
+    <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="177" formatCode="aaa"/>
+    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="179" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="180" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="181" formatCode="0_ "/>
+    <numFmt numFmtId="182" formatCode="0_ ;[Red]\-0\ "/>
+    <numFmt numFmtId="183" formatCode="0;&quot;△ &quot;0"/>
+    <numFmt numFmtId="184" formatCode="0;&quot;▲ &quot;0"/>
+    <numFmt numFmtId="185" formatCode="#,##0_);[Red]\(#,##0\)"/>
+    <numFmt numFmtId="186" formatCode="#,##0_);\(#,##0\)"/>
+    <numFmt numFmtId="187" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="188" formatCode="#,##0_ "/>
+    <numFmt numFmtId="189" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="190" formatCode="#,##0;&quot;△ &quot;#,##0"/>
+    <numFmt numFmtId="191" formatCode="#,##0;&quot;▲ &quot;#,##0"/>
+    <numFmt numFmtId="192" formatCode="#,##0.0_);[Red]\(#,##0.0\)"/>
+    <numFmt numFmtId="193" formatCode="#,##0.0_);\(#,##0.0\)"/>
+    <numFmt numFmtId="194" formatCode="#,##0.0;[Red]#,##0.0"/>
+    <numFmt numFmtId="195" formatCode="#,##0.0_ "/>
+    <numFmt numFmtId="196" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="197" formatCode="#,##0.0;&quot;△ &quot;#,##0.0"/>
+    <numFmt numFmtId="198" formatCode="#,##0.0;&quot;▲ &quot;#,##0.0"/>
+    <numFmt numFmtId="199" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
+    <numFmt numFmtId="200" formatCode="&quot;¥&quot;#,##0_);\(&quot;¥&quot;#,##0\)"/>
+    <numFmt numFmtId="201" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;#,##0"/>
+    <numFmt numFmtId="202" formatCode="&quot;¥&quot;#,##0.0_);[Red]\(&quot;¥&quot;#,##0.0\)"/>
+    <numFmt numFmtId="203" formatCode="&quot;¥&quot;#,##0.0_);\(&quot;¥&quot;#,##0.0\)"/>
+    <numFmt numFmtId="204" formatCode="&quot;¥&quot;#,##0.0;[Red]&quot;¥&quot;#,##0.0"/>
+    <numFmt numFmtId="205" formatCode="&quot;¥&quot;#,##0.0;&quot;¥&quot;\-#,##0.0"/>
+    <numFmt numFmtId="206" formatCode="&quot;¥&quot;#,##0.0;[Red]&quot;¥&quot;\-#,##0.0"/>
+    <numFmt numFmtId="207" formatCode="_ &quot;¥&quot;* #,##0.0_ ;_ &quot;¥&quot;* \-#,##0.0_ ;_ &quot;¥&quot;* &quot;-&quot;?_ ;_ @_ "/>
+    <numFmt numFmtId="208" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="209" formatCode="h:mm;@"/>
+    <numFmt numFmtId="210" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="211" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="212" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
+    <numFmt numFmtId="213" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="214" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="215" formatCode="m/d;@"/>
+    <numFmt numFmtId="216" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="217" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="218" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="219" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="220" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="221" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="222" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="223" formatCode="[$-409]mmmmm;@"/>
+    <numFmt numFmtId="224" formatCode="[$-409]mmmmm\-yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,11 +283,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="193" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="196" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="197" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="198" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="200" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="201" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="202" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="203" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="204" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="205" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="206" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="207" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="209" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="210" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="212" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="213" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="214" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="215" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="216" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="217" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="218" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="219" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="220" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="221" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="222" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="223" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="224" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -521,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -542,13 +683,13 @@
     </row>
     <row r="6" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -570,13 +711,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -585,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -597,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>600</v>
@@ -609,7 +750,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>700</v>
@@ -621,7 +762,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1500</v>
@@ -633,7 +774,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>400</v>
@@ -645,7 +786,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>500</v>
@@ -657,7 +798,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -669,7 +810,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>700</v>
@@ -681,7 +822,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>200</v>
@@ -693,7 +834,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>1000</v>
@@ -705,7 +846,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -729,19 +870,306 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="2">
+        <v>43831</v>
+      </c>
+      <c r="B2">
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C2" s="27">
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="D2" s="37">
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E2" s="40">
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <f>A$2</f>
+        <v>43831</v>
+      </c>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B12" si="0">$B2</f>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C3" s="28">
+        <f t="shared" ref="C3:C12" si="1">$B2</f>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="D3" s="38">
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E3" s="41">
+        <f t="shared" ref="E3:E18" si="2">$E2</f>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="4">
+        <f>A$2</f>
+        <v>43831</v>
+      </c>
+      <c r="B4" s="7">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C4" s="29">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="D4" s="39">
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E4" s="42">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <f>A$2</f>
+        <v>43831</v>
+      </c>
+      <c r="B5" s="8">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C5" s="30">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E5" s="43">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B6" s="9">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C6" s="27">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E6" s="44">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B7" s="10">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C7" s="31">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E7" s="45">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B8" s="11">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C8" s="32">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E8" s="46">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B9" s="12">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C9" s="33">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E9" s="47">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B10" s="13">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C10" s="34">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E10" s="48">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B11" s="14">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C11" s="35">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E11" s="49">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B12" s="15">
+        <f t="shared" si="0"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="C12" s="36">
+        <f t="shared" si="1"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E12" s="50">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B13" s="16">
+        <f t="shared" ref="B13:B23" si="3">$B12</f>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E13" s="51">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B14" s="17">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E14" s="52">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B15" s="18">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E15" s="53">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B16" s="19">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E16" s="54">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B17" s="20">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E17" s="55">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B18" s="21">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+      <c r="E18" s="56">
+        <f t="shared" si="2"/>
+        <v>43831.665983796294</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B19" s="22">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B20" s="23">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B21" s="24">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B22" s="25">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B23" s="26">
+        <f t="shared" si="3"/>
+        <v>-20000.099999999999</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>